<commit_message>
finished dcf and final valuation
</commit_message>
<xml_diff>
--- a/resources/Industry DCF Rules.xlsx
+++ b/resources/Industry DCF Rules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aidan\Documents\StockProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aidan\Documents\StockProject\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1978C7C6-92B3-4C31-9EA9-E200AC42F5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A6E7BB-ACF8-4C51-82A5-EBC8A7F1D0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AFEB0B20-5EAD-4FE5-8FAF-F4631C0D9A9A}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Sector</t>
   </si>
@@ -85,15 +85,9 @@
     <t>P/E Weight</t>
   </si>
   <si>
-    <t>P/S Weight</t>
-  </si>
-  <si>
     <t>P/B Weight</t>
   </si>
   <si>
-    <t>P/FFO Weight</t>
-  </si>
-  <si>
     <t>Financials</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>Healthcare</t>
   </si>
   <si>
-    <t>Consumer</t>
-  </si>
-  <si>
     <t>Energy</t>
   </si>
   <si>
@@ -127,23 +118,42 @@
     <t>Default</t>
   </si>
   <si>
-    <t>EV/EBITDA</t>
-  </si>
-  <si>
-    <t>EV/Revenue</t>
-  </si>
-  <si>
-    <t>P/E</t>
-  </si>
-  <si>
-    <t>P/B</t>
+    <t>EV/REVENUE Weight</t>
+  </si>
+  <si>
+    <t>Valuation Sum</t>
+  </si>
+  <si>
+    <t>Multiples Sum</t>
+  </si>
+  <si>
+    <t>Basic Materials</t>
+  </si>
+  <si>
+    <t>EV/EBITDA Weight</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Consumer Defensive</t>
+  </si>
+  <si>
+    <t>Consumer Cyclical</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,14 +179,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -508,23 +521,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF78FA4D-E017-4353-99B6-27358AB52EF4}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,24 +554,30 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -564,24 +586,32 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+      <c r="I2" s="1">
+        <f>SUM(C2:D2)</f>
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <f>SUM(E2:H2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>0.8</v>
@@ -590,24 +620,32 @@
         <v>0.2</v>
       </c>
       <c r="E3">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="F3">
-        <v>0.8</v>
+        <v>0.45</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I13" si="0">SUM(C3:D3)</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J13" si="1">SUM(E3:H3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>0.7</v>
@@ -619,21 +657,29 @@
         <v>0.4</v>
       </c>
       <c r="F4">
-        <v>0.6</v>
+        <v>0.45</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>0.6</v>
@@ -642,24 +688,32 @@
         <v>0.4</v>
       </c>
       <c r="E5">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>0.5</v>
@@ -668,24 +722,32 @@
         <v>0.5</v>
       </c>
       <c r="E6">
-        <v>0.3</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F6">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>0.7</v>
@@ -694,24 +756,32 @@
         <v>0.3</v>
       </c>
       <c r="E7">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F7">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>0.6</v>
@@ -720,24 +790,32 @@
         <v>0.4</v>
       </c>
       <c r="E8">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G8">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -746,24 +824,32 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>0.5</v>
@@ -772,78 +858,126 @@
         <v>0.5</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+      <c r="E11">
+        <v>0.5</v>
+      </c>
+      <c r="F11">
+        <v>0.3</v>
+      </c>
+      <c r="G11">
+        <v>0.15</v>
+      </c>
+      <c r="H11">
+        <v>0.05</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12">
+        <v>0.5</v>
+      </c>
+      <c r="E12">
+        <v>0.45</v>
+      </c>
+      <c r="F12">
+        <v>0.15</v>
+      </c>
+      <c r="G12">
+        <v>0.35</v>
+      </c>
+      <c r="H12">
+        <v>0.05</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+      <c r="E13">
+        <v>0.4</v>
+      </c>
+      <c r="F13">
+        <v>0.3</v>
+      </c>
+      <c r="G13">
+        <v>0.2</v>
+      </c>
+      <c r="H13">
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.99999999999999989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>